<commit_message>
Inclusion of Marsupial classifier list as a text file (tab-delimited)
</commit_message>
<xml_diff>
--- a/Data/Raw/Mars_classifier_list.xlsx
+++ b/Data/Raw/Mars_classifier_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github_Projects\Mars-shape\Data\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905C1666-C2CE-4044-8B26-E3D9BC482832}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B978832C-6A93-4F46-BCF8-1E10255D5A3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{CB33B8EB-E82A-4F25-B5F0-05EE142B67D4}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="77">
   <si>
     <t xml:space="preserve">Specimen </t>
   </si>
@@ -197,9 +197,6 @@
     <t>Terrestrial</t>
   </si>
   <si>
-    <t>Aquatic/Terrestrial</t>
-  </si>
-  <si>
     <t>Scansorial</t>
   </si>
   <si>
@@ -227,27 +224,15 @@
     <t>Peramelemorph</t>
   </si>
   <si>
-    <t>Carnivore-omnivore</t>
-  </si>
-  <si>
     <t>Omnivore</t>
   </si>
   <si>
-    <t>Carnivore-insectivore</t>
-  </si>
-  <si>
     <t>Insectivore</t>
   </si>
   <si>
     <t>Didelphid</t>
   </si>
   <si>
-    <t>Arboreal/Scansorial</t>
-  </si>
-  <si>
-    <t>Terrestrial/Scansorial</t>
-  </si>
-  <si>
     <t>Microbiod</t>
   </si>
   <si>
@@ -257,19 +242,25 @@
     <t>Carnivore</t>
   </si>
   <si>
-    <t>Insectivore-nectarivore</t>
-  </si>
-  <si>
-    <t>Herbivore-folivore</t>
-  </si>
-  <si>
     <t>Herbivore</t>
   </si>
   <si>
-    <t>Nectarivore-omnivore</t>
-  </si>
-  <si>
-    <t>Herbivore-omnivore</t>
+    <t>Aquatic_Terrestrial</t>
+  </si>
+  <si>
+    <t>Arboreal_Scansorial</t>
+  </si>
+  <si>
+    <t>Terrestrial_Scansorial</t>
+  </si>
+  <si>
+    <t>Insectivore_nectarivore</t>
+  </si>
+  <si>
+    <t>Herbivore_folivore</t>
+  </si>
+  <si>
+    <t>Nectarivore_omnivore</t>
   </si>
 </sst>
 </file>
@@ -633,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9645EE6-7301-44E8-A183-01981E697E95}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,7 +647,7 @@
         <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -667,10 +658,10 @@
         <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -681,10 +672,10 @@
         <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -692,13 +683,13 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -709,10 +700,10 @@
         <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -720,13 +711,13 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -737,10 +728,10 @@
         <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -748,13 +739,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -762,13 +753,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -779,10 +770,10 @@
         <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -790,13 +781,13 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -807,10 +798,10 @@
         <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -821,10 +812,10 @@
         <v>52</v>
       </c>
       <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" t="s">
         <v>67</v>
-      </c>
-      <c r="D13" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -835,10 +826,10 @@
         <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -849,10 +840,10 @@
         <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -863,10 +854,10 @@
         <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -877,10 +868,10 @@
         <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -891,10 +882,10 @@
         <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -905,10 +896,10 @@
         <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -919,10 +910,10 @@
         <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -930,13 +921,13 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -947,10 +938,10 @@
         <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -958,13 +949,13 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -972,13 +963,13 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -986,13 +977,13 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1000,13 +991,13 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1017,10 +1008,10 @@
         <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1031,10 +1022,10 @@
         <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1045,10 +1036,10 @@
         <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1056,13 +1047,13 @@
         <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1073,10 +1064,10 @@
         <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1087,10 +1078,10 @@
         <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1101,10 +1092,10 @@
         <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1115,10 +1106,10 @@
         <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1129,10 +1120,10 @@
         <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1143,10 +1134,10 @@
         <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1157,10 +1148,10 @@
         <v>52</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1171,10 +1162,10 @@
         <v>52</v>
       </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1182,13 +1173,13 @@
         <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D39" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1199,10 +1190,10 @@
         <v>54</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D40" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1213,10 +1204,10 @@
         <v>54</v>
       </c>
       <c r="C41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1227,10 +1218,10 @@
         <v>53</v>
       </c>
       <c r="C42" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1241,10 +1232,10 @@
         <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D43" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1255,10 +1246,10 @@
         <v>54</v>
       </c>
       <c r="C44" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1269,10 +1260,10 @@
         <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1283,10 +1274,10 @@
         <v>52</v>
       </c>
       <c r="C46" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D46" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1297,10 +1288,10 @@
         <v>52</v>
       </c>
       <c r="C47" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D47" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1308,13 +1299,13 @@
         <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C48" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1325,10 +1316,10 @@
         <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1339,10 +1330,10 @@
         <v>54</v>
       </c>
       <c r="C50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>